<commit_message>
How to export data to excel file
</commit_message>
<xml_diff>
--- a/wwwroot/UploadExcelFile/Cust_DummyData.xlsx
+++ b/wwwroot/UploadExcelFile/Cust_DummyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D00B780E-9EAE-4A9B-A5AA-AA43B6E4038E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5048482-0A31-4643-8045-DF3675988AEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13050" yWindow="4020" windowWidth="20955" windowHeight="10770" xr2:uid="{7B58B9E2-665E-4D99-9F6B-721B75D27B5A}"/>
+    <workbookView xWindow="6450" yWindow="7350" windowWidth="20955" windowHeight="10770" xr2:uid="{7B58B9E2-665E-4D99-9F6B-721B75D27B5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -503,10 +503,18 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>